<commit_message>
UPDATE[calc]: Range operator now working properly (#260)
</commit_message>
<xml_diff>
--- a/packages/calc/equalto_xlsx/tests/calc_tests/CHOOSE.xlsx
+++ b/packages/calc/equalto_xlsx/tests/calc_tests/CHOOSE.xlsx
@@ -1,28 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mateuszkopec/Sheets/packages/calc/equalto_xlsx/tests/calc_tests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolas/Dropbox/Excel files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24D0C231-09A9-AB49-8683-16C1345D53CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F365EB3-EE6F-6C45-A55B-8C0E7CDDB8F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34740" yWindow="1440" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CHOOSE" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>CHOOSE</t>
   </si>
@@ -72,15 +75,6 @@
   </si>
   <si>
     <t>Bolts</t>
-  </si>
-  <si>
-    <t>=SUM(A9:CHOOSE(2,A10,A11,A12))</t>
-  </si>
-  <si>
-    <t>not supported yet</t>
-  </si>
-  <si>
-    <t>=SUM(CHOOSE(2,A9:A10,A9:A11,A9:A12))</t>
   </si>
   <si>
     <t>=CHOOSE(-1, A4)</t>
@@ -305,7 +299,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -593,7 +587,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -603,8 +597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -623,13 +617,13 @@
         <v>1</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="F2" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G2" s="9" t="e">
         <f>1/0</f>
@@ -696,26 +690,26 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>23</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>15</v>
-      </c>
+      <c r="B10" s="5">
+        <f>SUM(A9:CHOOSE(2,A10,A11,A12))</f>
+        <v>68</v>
+      </c>
+      <c r="C10" s="8"/>
     </row>
     <row r="11" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>45</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>16</v>
+      <c r="B11" s="4">
+        <f>SUM(CHOOSE(2,A9:A10,A9:A11,A9:A12))</f>
+        <v>68</v>
       </c>
       <c r="C11" s="9">
         <f>SUM(CHOOSE(2,A10:A11,A10:A12,A10:A13))</f>
@@ -734,12 +728,12 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B16" s="9" t="e">
         <f>CHOOSE(-1, A4)</f>
@@ -748,7 +742,7 @@
     </row>
     <row r="17" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B17" s="9" t="e">
         <f>CHOOSE(0, A4)</f>
@@ -757,7 +751,7 @@
     </row>
     <row r="18" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B18" s="9" t="str">
         <f>CHOOSE(1, A4)</f>
@@ -766,7 +760,7 @@
     </row>
     <row r="19" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B19" s="9" t="e">
         <f>CHOOSE(2, A4)</f>
@@ -775,7 +769,7 @@
     </row>
     <row r="20" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B20" s="9" t="e">
         <f>CHOOSE("test", A4)</f>
@@ -784,7 +778,7 @@
     </row>
     <row r="21" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B21" s="9" t="e">
         <f>CHOOSE(FALSE, A4)</f>
@@ -793,7 +787,7 @@
     </row>
     <row r="22" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B22" s="9" t="str">
         <f>CHOOSE(TRUE, A4)</f>
@@ -802,7 +796,7 @@
     </row>
     <row r="23" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B23" s="9" t="e">
         <f>CHOOSE(A25:A27,A4,A5,A6)</f>
@@ -811,7 +805,7 @@
     </row>
     <row r="24" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B24" s="9" t="e">
         <f>CHOOSE(G2, A4)</f>
@@ -820,7 +814,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -828,7 +822,7 @@
         <v>1</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C27" s="9" t="str">
         <f>CHOOSE(A27, A4, A5, A6)</f>
@@ -840,7 +834,7 @@
         <v>2</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C28" s="9" t="str">
         <f>CHOOSE(A28, A4, A5, A6)</f>
@@ -852,7 +846,7 @@
         <v>3</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C29" s="9" t="str">
         <f>CHOOSE(A29, A4, A5, A6)</f>
@@ -861,12 +855,12 @@
     </row>
     <row r="31" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="32" spans="1:3" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B32" s="9" t="str">
         <f>CHOOSE(1.1,A4,A5)</f>
@@ -875,7 +869,7 @@
     </row>
     <row r="33" spans="1:2" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B33" s="9" t="str">
         <f>CHOOSE(1.9,A4,A5)</f>
@@ -884,12 +878,12 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="10" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B36" s="9">
         <f>CHOOSE(1, 0, G2)</f>
@@ -898,7 +892,7 @@
     </row>
     <row r="37" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B37" s="9" t="e">
         <f>CHOOSE(2, 0, G2)</f>
@@ -907,12 +901,12 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B40" s="9" t="str">
         <f>CHOOSE(2, B40, "Not a cycle")</f>

</xml_diff>